<commit_message>
fix(DocVal): add lab valid cond
</commit_message>
<xml_diff>
--- a/Step3-DocVal/DocVal_UniqueFields_5.8.24.xlsx
+++ b/Step3-DocVal/DocVal_UniqueFields_5.8.24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckhendry/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Dev\Javascript\Colleen Hendry\Step3-DocVal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{471E5B44-6E8A-5F44-BE66-21C8746E982A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D2871A-6AE2-497B-8C1F-D571052BBF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="3160" windowWidth="27240" windowHeight="16440" xr2:uid="{A5B32F58-7310-9445-80D8-D3D9FC316896}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A5B32F58-7310-9445-80D8-D3D9FC316896}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -510,7 +499,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -520,6 +509,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -626,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -637,6 +632,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -953,17 +949,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6518F2EB-FA4A-5542-8EF9-A117BD256579}">
   <dimension ref="A1:B170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="B159" sqref="B159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="121.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="121.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -971,23 +967,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="8">
         <v>112322885</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="8">
         <v>112322886</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -995,7 +991,7 @@
         <v>112323064</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1003,39 +999,39 @@
         <v>112323076</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="8">
         <v>112322887</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="8">
         <v>112322888</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="8">
         <v>112322889</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="8">
         <v>112323005</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -1043,23 +1039,23 @@
         <v>112323011</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="8">
         <v>112322893</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="8">
         <v>112322894</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1067,7 +1063,7 @@
         <v>112323017</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -1075,7 +1071,7 @@
         <v>112323030</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -1083,7 +1079,7 @@
         <v>112323033</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -1091,7 +1087,7 @@
         <v>112860482</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1099,7 +1095,7 @@
         <v>112860610</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
@@ -1107,15 +1103,15 @@
         <v>112860626</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="8">
         <v>112323036</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1123,7 +1119,7 @@
         <v>112323038</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -1131,7 +1127,7 @@
         <v>112377175</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
@@ -1139,7 +1135,7 @@
         <v>112431412</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
@@ -1147,7 +1143,7 @@
         <v>112323056</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -1155,7 +1151,7 @@
         <v>112323059</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -1163,15 +1159,15 @@
         <v>112323375</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="8">
         <v>112431416</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -1179,15 +1175,15 @@
         <v>112323077</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="8">
         <v>112377237</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
@@ -1195,15 +1191,15 @@
         <v>112323110</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="8">
         <v>112323129</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
@@ -1211,7 +1207,7 @@
         <v>112847017</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
@@ -1219,7 +1215,7 @@
         <v>112847019</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
@@ -1227,7 +1223,7 @@
         <v>112847046</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>32</v>
       </c>
@@ -1235,7 +1231,7 @@
         <v>112989680</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>33</v>
       </c>
@@ -1243,7 +1239,7 @@
         <v>112989681</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
@@ -1251,7 +1247,7 @@
         <v>112989699</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
@@ -1259,7 +1255,7 @@
         <v>112323140</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
@@ -1267,7 +1263,7 @@
         <v>112323143</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
@@ -1275,7 +1271,7 @@
         <v>112323145</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
@@ -1283,31 +1279,31 @@
         <v>112323226</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="8">
         <v>112323242</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="8">
         <v>112323265</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="8">
         <v>112323282</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>42</v>
       </c>
@@ -1315,31 +1311,31 @@
         <v>112323293</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="8">
         <v>112323331</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="8">
         <v>112323362</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B47" s="8">
         <v>112323371</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>46</v>
       </c>
@@ -1347,7 +1343,7 @@
         <v>112323454</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>47</v>
       </c>
@@ -1355,7 +1351,7 @@
         <v>112323455</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>48</v>
       </c>
@@ -1363,15 +1359,15 @@
         <v>112323458</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51" s="8">
         <v>112431884</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>49</v>
       </c>
@@ -1379,7 +1375,7 @@
         <v>112323597</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>50</v>
       </c>
@@ -1387,7 +1383,7 @@
         <v>112323599</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>51</v>
       </c>
@@ -1395,23 +1391,23 @@
         <v>112375535</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B55" s="8">
         <v>112430683</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B56" s="8">
         <v>113034625</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>54</v>
       </c>
@@ -1419,7 +1415,7 @@
         <v>112323602</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>55</v>
       </c>
@@ -1427,15 +1423,15 @@
         <v>112323619</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B59" s="8">
         <v>112827021</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
@@ -1443,7 +1439,7 @@
         <v>112323620</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>58</v>
       </c>
@@ -1451,7 +1447,7 @@
         <v>112375817</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>59</v>
       </c>
@@ -1459,15 +1455,15 @@
         <v>112375819</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B63" s="8">
         <v>112323725</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>61</v>
       </c>
@@ -1475,7 +1471,7 @@
         <v>112645327</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>62</v>
       </c>
@@ -1483,7 +1479,7 @@
         <v>112645328</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>63</v>
       </c>
@@ -1491,7 +1487,7 @@
         <v>112645329</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>64</v>
       </c>
@@ -1499,7 +1495,7 @@
         <v>112323750</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>65</v>
       </c>
@@ -1507,7 +1503,7 @@
         <v>112323782</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>66</v>
       </c>
@@ -1515,7 +1511,7 @@
         <v>112323785</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>67</v>
       </c>
@@ -1523,7 +1519,7 @@
         <v>112323786</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>68</v>
       </c>
@@ -1531,39 +1527,39 @@
         <v>112375880</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="4">
+      <c r="B72" s="8">
         <v>112323807</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B73" s="4">
+      <c r="B73" s="8">
         <v>112323837</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B74" s="4">
+      <c r="B74" s="8">
         <v>112323854</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B75" s="4">
+      <c r="B75" s="8">
         <v>113034731</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>71</v>
       </c>
@@ -1571,7 +1567,7 @@
         <v>113035642</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>70</v>
       </c>
@@ -1579,7 +1575,7 @@
         <v>113037492</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>72</v>
       </c>
@@ -1587,7 +1583,7 @@
         <v>113035644</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>73</v>
       </c>
@@ -1595,7 +1591,7 @@
         <v>113037493</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>74</v>
       </c>
@@ -1603,7 +1599,7 @@
         <v>112323923</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>75</v>
       </c>
@@ -1611,7 +1607,7 @@
         <v>112323926</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>70</v>
       </c>
@@ -1619,7 +1615,7 @@
         <v>112323944</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>76</v>
       </c>
@@ -1627,7 +1623,7 @@
         <v>112483915</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>77</v>
       </c>
@@ -1635,7 +1631,7 @@
         <v>112323945</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>78</v>
       </c>
@@ -1643,7 +1639,7 @@
         <v>112483916</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>79</v>
       </c>
@@ -1651,7 +1647,7 @@
         <v>112648846</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>59</v>
       </c>
@@ -1659,7 +1655,7 @@
         <v>113138061</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>80</v>
       </c>
@@ -1667,23 +1663,23 @@
         <v>112323639</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B89" s="4">
+      <c r="B89" s="8">
         <v>112641343</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B90" s="4">
+      <c r="B90" s="8">
         <v>112641345</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>83</v>
       </c>
@@ -1691,7 +1687,7 @@
         <v>112641482</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>84</v>
       </c>
@@ -1699,15 +1695,15 @@
         <v>112642137</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B93" s="4">
+      <c r="B93" s="8">
         <v>112375836</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>86</v>
       </c>
@@ -1715,7 +1711,7 @@
         <v>112323656</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>87</v>
       </c>
@@ -1723,7 +1719,7 @@
         <v>112323672</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>88</v>
       </c>
@@ -1731,7 +1727,7 @@
         <v>112323673</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>50</v>
       </c>
@@ -1739,7 +1735,7 @@
         <v>112323674</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>68</v>
       </c>
@@ -1747,7 +1743,7 @@
         <v>112375545</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>89</v>
       </c>
@@ -1755,15 +1751,15 @@
         <v>112323684</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B100" s="4">
+      <c r="B100" s="8">
         <v>112323692</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>45</v>
       </c>
@@ -1771,39 +1767,39 @@
         <v>112323695</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B102" s="4">
+      <c r="B102" s="8">
         <v>112324474</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B103" s="4">
+      <c r="B103" s="8">
         <v>113121720</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B104" s="4">
+      <c r="B104" s="8">
         <v>113121728</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B105" s="4">
+      <c r="B105" s="8">
         <v>113121725</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>90</v>
       </c>
@@ -1811,7 +1807,7 @@
         <v>113037493</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>91</v>
       </c>
@@ -1819,7 +1815,7 @@
         <v>112323923</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>92</v>
       </c>
@@ -1827,7 +1823,7 @@
         <v>112323704</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>93</v>
       </c>
@@ -1835,7 +1831,7 @@
         <v>112323705</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>94</v>
       </c>
@@ -1843,7 +1839,7 @@
         <v>112648834</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>59</v>
       </c>
@@ -1851,7 +1847,7 @@
         <v>112648843</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>95</v>
       </c>
@@ -1859,7 +1855,7 @@
         <v>112430828</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>96</v>
       </c>
@@ -1867,7 +1863,7 @@
         <v>112430830</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>97</v>
       </c>
@@ -1875,7 +1871,7 @@
         <v>112430870</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>98</v>
       </c>
@@ -1883,7 +1879,7 @@
         <v>112430902</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>99</v>
       </c>
@@ -1891,7 +1887,7 @@
         <v>112431042</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>100</v>
       </c>
@@ -1899,7 +1895,7 @@
         <v>112431208</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>101</v>
       </c>
@@ -1907,7 +1903,7 @@
         <v>112431213</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>102</v>
       </c>
@@ -1915,7 +1911,7 @@
         <v>112431214</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>73</v>
       </c>
@@ -1923,7 +1919,7 @@
         <v>113049411</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>103</v>
       </c>
@@ -1931,7 +1927,7 @@
         <v>113048802</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>104</v>
       </c>
@@ -1939,7 +1935,7 @@
         <v>112431241</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>105</v>
       </c>
@@ -1947,7 +1943,7 @@
         <v>112431243</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>106</v>
       </c>
@@ -1955,7 +1951,7 @@
         <v>112761604</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>107</v>
       </c>
@@ -1963,7 +1959,7 @@
         <v>112761651</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>108</v>
       </c>
@@ -1971,7 +1967,7 @@
         <v>112761654</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>109</v>
       </c>
@@ -1979,7 +1975,7 @@
         <v>112761704</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>110</v>
       </c>
@@ -1987,7 +1983,7 @@
         <v>112761706</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>111</v>
       </c>
@@ -1995,7 +1991,7 @@
         <v>112761709</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>112</v>
       </c>
@@ -2003,7 +1999,7 @@
         <v>112431216</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>113</v>
       </c>
@@ -2011,7 +2007,7 @@
         <v>112991048</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>114</v>
       </c>
@@ -2019,7 +2015,7 @@
         <v>112991049</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>115</v>
       </c>
@@ -2027,7 +2023,7 @@
         <v>112990091</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>116</v>
       </c>
@@ -2035,7 +2031,7 @@
         <v>112761221</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>117</v>
       </c>
@@ -2043,7 +2039,7 @@
         <v>112761457</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>118</v>
       </c>
@@ -2051,7 +2047,7 @@
         <v>113121752</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>119</v>
       </c>
@@ -2059,7 +2055,7 @@
         <v>112761524</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>120</v>
       </c>
@@ -2067,7 +2063,7 @@
         <v>112761475</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>121</v>
       </c>
@@ -2075,7 +2071,7 @@
         <v>112761476</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>122</v>
       </c>
@@ -2083,7 +2079,7 @@
         <v>112431237</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>123</v>
       </c>
@@ -2091,7 +2087,7 @@
         <v>112431239</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>128</v>
       </c>
@@ -2099,7 +2095,7 @@
         <v>112431272</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>129</v>
       </c>
@@ -2107,7 +2103,7 @@
         <v>112431280</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>130</v>
       </c>
@@ -2115,7 +2111,7 @@
         <v>112431282</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>131</v>
       </c>
@@ -2123,7 +2119,7 @@
         <v>112431283</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>132</v>
       </c>
@@ -2131,7 +2127,7 @@
         <v>112431291</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>133</v>
       </c>
@@ -2139,7 +2135,7 @@
         <v>112431360</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>124</v>
       </c>
@@ -2147,7 +2143,7 @@
         <v>112431245</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>125</v>
       </c>
@@ -2155,7 +2151,7 @@
         <v>112431280</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>126</v>
       </c>
@@ -2163,7 +2159,7 @@
         <v>112431282</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>127</v>
       </c>
@@ -2171,7 +2167,7 @@
         <v>112431283</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>148</v>
       </c>
@@ -2179,7 +2175,7 @@
         <v>113136848</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>59</v>
       </c>
@@ -2187,7 +2183,7 @@
         <v>112648848</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>134</v>
       </c>
@@ -2195,7 +2191,7 @@
         <v>112342179</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>135</v>
       </c>
@@ -2203,7 +2199,7 @@
         <v>112481721</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>136</v>
       </c>
@@ -2211,15 +2207,15 @@
         <v>112481731</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B157" s="4">
+      <c r="B157" s="8">
         <v>112730381</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>138</v>
       </c>
@@ -2227,15 +2223,15 @@
         <v>112481734</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B159" s="4">
+      <c r="B159" s="8">
         <v>112730438</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>140</v>
       </c>
@@ -2243,7 +2239,7 @@
         <v>112481736</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>141</v>
       </c>
@@ -2251,7 +2247,7 @@
         <v>112484045</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>142</v>
       </c>
@@ -2259,7 +2255,7 @@
         <v>112481804</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>143</v>
       </c>
@@ -2267,7 +2263,7 @@
         <v>112342184</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>144</v>
       </c>
@@ -2275,7 +2271,7 @@
         <v>112607191</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>145</v>
       </c>
@@ -2283,7 +2279,7 @@
         <v>112481953</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>146</v>
       </c>
@@ -2291,7 +2287,7 @@
         <v>112481954</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>145</v>
       </c>
@@ -2299,7 +2295,7 @@
         <v>112481970</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>146</v>
       </c>
@@ -2307,7 +2303,7 @@
         <v>112481972</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>147</v>
       </c>
@@ -2315,7 +2311,7 @@
         <v>112322910</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="6"/>
       <c r="B170" s="7"/>
     </row>

</xml_diff>